<commit_message>
Update sidebar saving logic
</commit_message>
<xml_diff>
--- a/PC Template 2.xlsx
+++ b/PC Template 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anaconda3\PC-Template-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBC1B5E-4796-4E75-8E9F-9C9EB4B12397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62742E31-542F-4007-B5CD-8FD6EACA1FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3105D93-4F2D-4261-B669-05F183F1BD78}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{C3105D93-4F2D-4261-B669-05F183F1BD78}"/>
   </bookViews>
   <sheets>
     <sheet name="DETAILS" sheetId="18" r:id="rId1"/>
@@ -2168,6 +2168,45 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2181,12 +2220,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2195,38 +2228,32 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2234,15 +2261,63 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="54" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2252,113 +2327,38 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2899,67 +2899,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{842912D2-8274-582B-FEE6-B356DB5CDEBA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="53340" y="0"/>
-          <a:ext cx="754380" cy="716280"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
@@ -3065,266 +3004,11 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>83821</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>482264</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 1" descr="~AUT0000">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{290BA305-51CA-B596-09D4-53FDD649DB87}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:lum bright="12000" contrast="60000"/>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8884920" y="83821"/>
-          <a:ext cx="634664" cy="624840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBE7126B-62A3-445B-DEE2-ECD4C15379E3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="50800" y="38100"/>
-          <a:ext cx="927100" cy="736600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:sysClr val="window" lastClr="FFFFFF"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100" kern="1200"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CE5B438-4277-F23C-CD31-76C2932FFD09}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9372600" y="0"/>
-          <a:ext cx="850900" cy="736600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:sysClr val="window" lastClr="FFFFFF"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100" kern="1200"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52AD5391-96ED-4A6F-81A9-8230FF40E8C4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="53340" y="0"/>
-          <a:ext cx="815340" cy="716280"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -3431,200 +3115,6 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>83821</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>482264</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 1" descr="~AUT0000">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93AC2742-4542-45D8-AA3C-3DE9A3101735}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:lum bright="12000" contrast="60000"/>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9624060" y="83821"/>
-          <a:ext cx="634664" cy="624840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F188AA28-F62F-4FCE-98E1-19F3AC9F30DF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="50800" y="38100"/>
-          <a:ext cx="932180" cy="736600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:sysClr val="window" lastClr="FFFFFF"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100" kern="1200"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B727ED92-FBAC-47EC-8B13-3DD003CBC1C8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9375140" y="0"/>
-          <a:ext cx="845820" cy="741680"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:sysClr val="window" lastClr="FFFFFF"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100" kern="1200"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4702,7 +4192,7 @@
   </sheetPr>
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5269,142 +4759,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="237"/>
-      <c r="B1" s="237"/>
-      <c r="C1" s="237"/>
-      <c r="D1" s="237"/>
+      <c r="A1" s="243"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="237"/>
-      <c r="B2" s="237"/>
-      <c r="C2" s="237"/>
-      <c r="D2" s="237"/>
+      <c r="A2" s="243"/>
+      <c r="B2" s="243"/>
+      <c r="C2" s="243"/>
+      <c r="D2" s="243"/>
     </row>
     <row r="3" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A3" s="237"/>
-      <c r="B3" s="237"/>
-      <c r="C3" s="237"/>
-      <c r="D3" s="237"/>
+      <c r="A3" s="243"/>
+      <c r="B3" s="243"/>
+      <c r="C3" s="243"/>
+      <c r="D3" s="243"/>
     </row>
     <row r="4" spans="1:4" s="28" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="237"/>
-      <c r="B4" s="237"/>
-      <c r="C4" s="237"/>
-      <c r="D4" s="237"/>
+      <c r="A4" s="243"/>
+      <c r="B4" s="243"/>
+      <c r="C4" s="243"/>
+      <c r="D4" s="243"/>
     </row>
     <row r="5" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A5" s="237"/>
-      <c r="B5" s="237"/>
-      <c r="C5" s="237"/>
-      <c r="D5" s="237"/>
+      <c r="A5" s="243"/>
+      <c r="B5" s="243"/>
+      <c r="C5" s="243"/>
+      <c r="D5" s="243"/>
     </row>
     <row r="6" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A6" s="237"/>
-      <c r="B6" s="237"/>
-      <c r="C6" s="237"/>
-      <c r="D6" s="237"/>
+      <c r="A6" s="243"/>
+      <c r="B6" s="243"/>
+      <c r="C6" s="243"/>
+      <c r="D6" s="243"/>
     </row>
     <row r="7" spans="1:4" s="28" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="238" t="str">
+      <c r="A7" s="244" t="str">
         <f>'PC 1'!B57 &amp; "                                                                             " &amp; 'PC 1'!B58</f>
         <v>0                                                                             0</v>
       </c>
-      <c r="B7" s="238"/>
-      <c r="C7" s="238"/>
-      <c r="D7" s="238"/>
+      <c r="B7" s="244"/>
+      <c r="C7" s="244"/>
+      <c r="D7" s="244"/>
     </row>
     <row r="8" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A8" s="239"/>
-      <c r="B8" s="239"/>
-      <c r="C8" s="239"/>
-      <c r="D8" s="239"/>
+      <c r="A8" s="238"/>
+      <c r="B8" s="238"/>
+      <c r="C8" s="238"/>
+      <c r="D8" s="238"/>
     </row>
     <row r="9" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A9" s="238">
+      <c r="A9" s="244">
         <f>'PC 1'!B59</f>
         <v>0</v>
       </c>
-      <c r="B9" s="238"/>
-      <c r="C9" s="238"/>
-      <c r="D9" s="238"/>
+      <c r="B9" s="244"/>
+      <c r="C9" s="244"/>
+      <c r="D9" s="244"/>
     </row>
     <row r="10" spans="1:4" s="28" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="236" t="str">
+      <c r="A10" s="237" t="str">
         <f>'PC 1'!B60</f>
         <v>,</v>
       </c>
-      <c r="B10" s="236"/>
-      <c r="C10" s="236"/>
-      <c r="D10" s="236"/>
+      <c r="B10" s="237"/>
+      <c r="C10" s="237"/>
+      <c r="D10" s="237"/>
     </row>
     <row r="11" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A11" s="236">
+      <c r="A11" s="237">
         <f>'PC 1'!B61</f>
         <v>0</v>
       </c>
-      <c r="B11" s="236"/>
-      <c r="C11" s="236"/>
-      <c r="D11" s="236"/>
+      <c r="B11" s="237"/>
+      <c r="C11" s="237"/>
+      <c r="D11" s="237"/>
     </row>
     <row r="12" spans="1:4" s="28" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="236">
+      <c r="A12" s="237">
         <f>'PC 1'!B62</f>
         <v>0</v>
       </c>
-      <c r="B12" s="236"/>
-      <c r="C12" s="236"/>
-      <c r="D12" s="236"/>
+      <c r="B12" s="237"/>
+      <c r="C12" s="237"/>
+      <c r="D12" s="237"/>
     </row>
     <row r="13" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A13" s="236">
+      <c r="A13" s="237">
         <f>'PC 1'!B63</f>
         <v>0</v>
       </c>
-      <c r="B13" s="236"/>
-      <c r="C13" s="236"/>
-      <c r="D13" s="236"/>
+      <c r="B13" s="237"/>
+      <c r="C13" s="237"/>
+      <c r="D13" s="237"/>
     </row>
     <row r="14" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A14" s="236"/>
-      <c r="B14" s="236"/>
-      <c r="C14" s="236"/>
-      <c r="D14" s="236"/>
+      <c r="A14" s="237"/>
+      <c r="B14" s="237"/>
+      <c r="C14" s="237"/>
+      <c r="D14" s="237"/>
     </row>
     <row r="15" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A15" s="239" t="s">
+      <c r="A15" s="238" t="s">
         <v>152</v>
       </c>
-      <c r="B15" s="239"/>
-      <c r="C15" s="239"/>
-      <c r="D15" s="239"/>
+      <c r="B15" s="238"/>
+      <c r="C15" s="238"/>
+      <c r="D15" s="238"/>
     </row>
     <row r="16" spans="1:4" s="28" customFormat="1" ht="67.2" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="241" t="str">
+      <c r="A16" s="239" t="str">
         <f>'PC 1'!B24 &amp; " " &amp; "&amp;" &amp; " " &amp;'PC 2'!B24 &amp; "."</f>
         <v>0 &amp; 0.</v>
       </c>
-      <c r="B16" s="241"/>
-      <c r="C16" s="241"/>
-      <c r="D16" s="241"/>
+      <c r="B16" s="239"/>
+      <c r="C16" s="239"/>
+      <c r="D16" s="239"/>
     </row>
     <row r="17" spans="1:10" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
       <c r="A17" s="30"/>
       <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:10" s="28" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="242" t="str">
+      <c r="A18" s="240" t="str">
         <f>"         I am directed to refer to your letter Ref. No. "&amp;'PC 1'!B64&amp;" &amp; "&amp;'PC 2'!B64&amp;" dated "&amp;'PC 1'!B65&amp;" &amp; "&amp;'PC 2'!B65&amp;" respectively, on the above subject and inform you that approval for the Pre-payment Certificates has been granted in the following sums:"</f>
         <v xml:space="preserve">         I am directed to refer to your letter Ref. No. 0 &amp; 0 dated 0 &amp; 0 respectively, on the above subject and inform you that approval for the Pre-payment Certificates has been granted in the following sums:</v>
       </c>
-      <c r="B18" s="242"/>
-      <c r="C18" s="242"/>
-      <c r="D18" s="242"/>
+      <c r="B18" s="240"/>
+      <c r="C18" s="240"/>
+      <c r="D18" s="240"/>
     </row>
     <row r="19" spans="1:10" s="28" customFormat="1" ht="22.95" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="243"/>
-      <c r="B19" s="243"/>
-      <c r="C19" s="243"/>
-      <c r="D19" s="243"/>
+      <c r="A19" s="241"/>
+      <c r="B19" s="241"/>
+      <c r="C19" s="241"/>
+      <c r="D19" s="241"/>
     </row>
     <row r="20" spans="1:10" s="28" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="53" t="s">
@@ -5460,48 +4950,48 @@
       <c r="C23" s="50"/>
     </row>
     <row r="24" spans="1:10" s="28" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="244" t="s">
+      <c r="A24" s="242" t="s">
         <v>153</v>
       </c>
-      <c r="B24" s="244"/>
-      <c r="C24" s="244"/>
-      <c r="D24" s="244"/>
+      <c r="B24" s="242"/>
+      <c r="C24" s="242"/>
+      <c r="D24" s="242"/>
     </row>
     <row r="25" spans="1:10" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A25" s="236"/>
-      <c r="B25" s="236"/>
-      <c r="C25" s="236"/>
-      <c r="D25" s="236"/>
+      <c r="A25" s="237"/>
+      <c r="B25" s="237"/>
+      <c r="C25" s="237"/>
+      <c r="D25" s="237"/>
     </row>
     <row r="26" spans="1:10" s="28" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A26" s="236" t="s">
+      <c r="A26" s="237" t="s">
         <v>154</v>
       </c>
-      <c r="B26" s="236"/>
-      <c r="C26" s="236"/>
-      <c r="D26" s="236"/>
+      <c r="B26" s="237"/>
+      <c r="C26" s="237"/>
+      <c r="D26" s="237"/>
     </row>
     <row r="27" spans="1:10" s="28" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A27" s="236"/>
-      <c r="B27" s="236"/>
-      <c r="C27" s="236"/>
-      <c r="D27" s="236"/>
+      <c r="A27" s="237"/>
+      <c r="B27" s="237"/>
+      <c r="C27" s="237"/>
+      <c r="D27" s="237"/>
     </row>
     <row r="28" spans="1:10" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A28" s="240" t="s">
+      <c r="A28" s="236" t="s">
         <v>156</v>
       </c>
-      <c r="B28" s="240"/>
-      <c r="C28" s="240"/>
-      <c r="D28" s="240"/>
+      <c r="B28" s="236"/>
+      <c r="C28" s="236"/>
+      <c r="D28" s="236"/>
     </row>
     <row r="29" spans="1:10" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A29" s="240" t="s">
+      <c r="A29" s="236" t="s">
         <v>155</v>
       </c>
-      <c r="B29" s="240"/>
-      <c r="C29" s="240"/>
-      <c r="D29" s="240"/>
+      <c r="B29" s="236"/>
+      <c r="C29" s="236"/>
+      <c r="D29" s="236"/>
     </row>
     <row r="30" spans="1:10" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
       <c r="A30" s="31"/>
@@ -5526,6 +5016,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A14:D14"/>
@@ -5538,18 +5040,6 @@
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -5577,142 +5067,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="237"/>
-      <c r="B1" s="237"/>
-      <c r="C1" s="237"/>
-      <c r="D1" s="237"/>
+      <c r="A1" s="243"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="237"/>
-      <c r="B2" s="237"/>
-      <c r="C2" s="237"/>
-      <c r="D2" s="237"/>
+      <c r="A2" s="243"/>
+      <c r="B2" s="243"/>
+      <c r="C2" s="243"/>
+      <c r="D2" s="243"/>
     </row>
     <row r="3" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A3" s="237"/>
-      <c r="B3" s="237"/>
-      <c r="C3" s="237"/>
-      <c r="D3" s="237"/>
+      <c r="A3" s="243"/>
+      <c r="B3" s="243"/>
+      <c r="C3" s="243"/>
+      <c r="D3" s="243"/>
     </row>
     <row r="4" spans="1:4" s="28" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="237"/>
-      <c r="B4" s="237"/>
-      <c r="C4" s="237"/>
-      <c r="D4" s="237"/>
+      <c r="A4" s="243"/>
+      <c r="B4" s="243"/>
+      <c r="C4" s="243"/>
+      <c r="D4" s="243"/>
     </row>
     <row r="5" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A5" s="237"/>
-      <c r="B5" s="237"/>
-      <c r="C5" s="237"/>
-      <c r="D5" s="237"/>
+      <c r="A5" s="243"/>
+      <c r="B5" s="243"/>
+      <c r="C5" s="243"/>
+      <c r="D5" s="243"/>
     </row>
     <row r="6" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A6" s="237"/>
-      <c r="B6" s="237"/>
-      <c r="C6" s="237"/>
-      <c r="D6" s="237"/>
+      <c r="A6" s="243"/>
+      <c r="B6" s="243"/>
+      <c r="C6" s="243"/>
+      <c r="D6" s="243"/>
     </row>
     <row r="7" spans="1:4" s="28" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="238" t="str">
+      <c r="A7" s="244" t="str">
         <f>'PC 1'!B57 &amp; "                                                                             " &amp; 'PC 1'!B58</f>
         <v>0                                                                             0</v>
       </c>
-      <c r="B7" s="238"/>
-      <c r="C7" s="238"/>
-      <c r="D7" s="238"/>
+      <c r="B7" s="244"/>
+      <c r="C7" s="244"/>
+      <c r="D7" s="244"/>
     </row>
     <row r="8" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A8" s="239"/>
-      <c r="B8" s="239"/>
-      <c r="C8" s="239"/>
-      <c r="D8" s="239"/>
+      <c r="A8" s="238"/>
+      <c r="B8" s="238"/>
+      <c r="C8" s="238"/>
+      <c r="D8" s="238"/>
     </row>
     <row r="9" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A9" s="238">
+      <c r="A9" s="244">
         <f>'PC 1'!B59</f>
         <v>0</v>
       </c>
-      <c r="B9" s="238"/>
-      <c r="C9" s="238"/>
-      <c r="D9" s="238"/>
+      <c r="B9" s="244"/>
+      <c r="C9" s="244"/>
+      <c r="D9" s="244"/>
     </row>
     <row r="10" spans="1:4" s="28" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="236" t="str">
+      <c r="A10" s="237" t="str">
         <f>'PC 1'!B60</f>
         <v>,</v>
       </c>
-      <c r="B10" s="236"/>
-      <c r="C10" s="236"/>
-      <c r="D10" s="236"/>
+      <c r="B10" s="237"/>
+      <c r="C10" s="237"/>
+      <c r="D10" s="237"/>
     </row>
     <row r="11" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A11" s="236">
+      <c r="A11" s="237">
         <f>'PC 1'!B61</f>
         <v>0</v>
       </c>
-      <c r="B11" s="236"/>
-      <c r="C11" s="236"/>
-      <c r="D11" s="236"/>
+      <c r="B11" s="237"/>
+      <c r="C11" s="237"/>
+      <c r="D11" s="237"/>
     </row>
     <row r="12" spans="1:4" s="28" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="236">
+      <c r="A12" s="237">
         <f>'PC 1'!B62</f>
         <v>0</v>
       </c>
-      <c r="B12" s="236"/>
-      <c r="C12" s="236"/>
-      <c r="D12" s="236"/>
+      <c r="B12" s="237"/>
+      <c r="C12" s="237"/>
+      <c r="D12" s="237"/>
     </row>
     <row r="13" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A13" s="236">
+      <c r="A13" s="237">
         <f>'PC 1'!B63</f>
         <v>0</v>
       </c>
-      <c r="B13" s="236"/>
-      <c r="C13" s="236"/>
-      <c r="D13" s="236"/>
+      <c r="B13" s="237"/>
+      <c r="C13" s="237"/>
+      <c r="D13" s="237"/>
     </row>
     <row r="14" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A14" s="236"/>
-      <c r="B14" s="236"/>
-      <c r="C14" s="236"/>
-      <c r="D14" s="236"/>
+      <c r="A14" s="237"/>
+      <c r="B14" s="237"/>
+      <c r="C14" s="237"/>
+      <c r="D14" s="237"/>
     </row>
     <row r="15" spans="1:4" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A15" s="239" t="s">
+      <c r="A15" s="238" t="s">
         <v>152</v>
       </c>
-      <c r="B15" s="239"/>
-      <c r="C15" s="239"/>
-      <c r="D15" s="239"/>
+      <c r="B15" s="238"/>
+      <c r="C15" s="238"/>
+      <c r="D15" s="238"/>
     </row>
     <row r="16" spans="1:4" s="28" customFormat="1" ht="67.2" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="241" t="str">
+      <c r="A16" s="239" t="str">
         <f>'PC 1'!B24 &amp; " " &amp; "&amp;" &amp; " " &amp;'PC 2'!B24 &amp; "."</f>
         <v>0 &amp; 0.</v>
       </c>
-      <c r="B16" s="241"/>
-      <c r="C16" s="241"/>
-      <c r="D16" s="241"/>
+      <c r="B16" s="239"/>
+      <c r="C16" s="239"/>
+      <c r="D16" s="239"/>
     </row>
     <row r="17" spans="1:10" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
       <c r="A17" s="30"/>
       <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:10" s="28" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="242" t="str">
+      <c r="A18" s="240" t="str">
         <f>"         I am directed to refer to your letter Ref. No. "&amp;'PC 1'!B64 &amp;" dated "&amp;'PC 1'!B65&amp;", on the above subject and inform you that approval for the Pre-payment Certificates has been granted in the following sums:"</f>
         <v xml:space="preserve">         I am directed to refer to your letter Ref. No. 0 dated 0, on the above subject and inform you that approval for the Pre-payment Certificates has been granted in the following sums:</v>
       </c>
-      <c r="B18" s="242"/>
-      <c r="C18" s="242"/>
-      <c r="D18" s="242"/>
+      <c r="B18" s="240"/>
+      <c r="C18" s="240"/>
+      <c r="D18" s="240"/>
     </row>
     <row r="19" spans="1:10" s="28" customFormat="1" ht="22.95" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="243"/>
-      <c r="B19" s="243"/>
-      <c r="C19" s="243"/>
-      <c r="D19" s="243"/>
+      <c r="A19" s="241"/>
+      <c r="B19" s="241"/>
+      <c r="C19" s="241"/>
+      <c r="D19" s="241"/>
     </row>
     <row r="20" spans="1:10" s="28" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="53" t="s">
@@ -5768,48 +5258,48 @@
       <c r="C23" s="50"/>
     </row>
     <row r="24" spans="1:10" s="28" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="244" t="s">
+      <c r="A24" s="242" t="s">
         <v>153</v>
       </c>
-      <c r="B24" s="244"/>
-      <c r="C24" s="244"/>
-      <c r="D24" s="244"/>
+      <c r="B24" s="242"/>
+      <c r="C24" s="242"/>
+      <c r="D24" s="242"/>
     </row>
     <row r="25" spans="1:10" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A25" s="236"/>
-      <c r="B25" s="236"/>
-      <c r="C25" s="236"/>
-      <c r="D25" s="236"/>
+      <c r="A25" s="237"/>
+      <c r="B25" s="237"/>
+      <c r="C25" s="237"/>
+      <c r="D25" s="237"/>
     </row>
     <row r="26" spans="1:10" s="28" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A26" s="236" t="s">
+      <c r="A26" s="237" t="s">
         <v>154</v>
       </c>
-      <c r="B26" s="236"/>
-      <c r="C26" s="236"/>
-      <c r="D26" s="236"/>
+      <c r="B26" s="237"/>
+      <c r="C26" s="237"/>
+      <c r="D26" s="237"/>
     </row>
     <row r="27" spans="1:10" s="28" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A27" s="236"/>
-      <c r="B27" s="236"/>
-      <c r="C27" s="236"/>
-      <c r="D27" s="236"/>
+      <c r="A27" s="237"/>
+      <c r="B27" s="237"/>
+      <c r="C27" s="237"/>
+      <c r="D27" s="237"/>
     </row>
     <row r="28" spans="1:10" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A28" s="240" t="s">
+      <c r="A28" s="236" t="s">
         <v>156</v>
       </c>
-      <c r="B28" s="240"/>
-      <c r="C28" s="240"/>
-      <c r="D28" s="240"/>
+      <c r="B28" s="236"/>
+      <c r="C28" s="236"/>
+      <c r="D28" s="236"/>
     </row>
     <row r="29" spans="1:10" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
-      <c r="A29" s="240" t="s">
+      <c r="A29" s="236" t="s">
         <v>155</v>
       </c>
-      <c r="B29" s="240"/>
-      <c r="C29" s="240"/>
-      <c r="D29" s="240"/>
+      <c r="B29" s="236"/>
+      <c r="C29" s="236"/>
+      <c r="D29" s="236"/>
     </row>
     <row r="30" spans="1:10" s="28" customFormat="1" ht="23.4" x14ac:dyDescent="0.6">
       <c r="A30" s="31"/>
@@ -5834,6 +5324,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A14:D14"/>
@@ -5846,18 +5348,6 @@
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -7522,7 +7012,7 @@
   </sheetPr>
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A4" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C26" sqref="C26:I26"/>
     </sheetView>
   </sheetViews>
@@ -7545,79 +7035,79 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="188">
+      <c r="A2" s="180">
         <f>'PC 1'!B55</f>
         <v>0</v>
       </c>
-      <c r="B2" s="188"/>
-      <c r="C2" s="188"/>
-      <c r="D2" s="188"/>
-      <c r="E2" s="188"/>
-      <c r="F2" s="188"/>
-      <c r="G2" s="188"/>
-      <c r="H2" s="188"/>
-      <c r="I2" s="188"/>
+      <c r="B2" s="180"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
+      <c r="I2" s="180"/>
     </row>
     <row r="3" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="199" t="s">
+      <c r="A3" s="181" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="199"/>
-      <c r="C3" s="199"/>
-      <c r="D3" s="199"/>
-      <c r="E3" s="199"/>
-      <c r="F3" s="199"/>
-      <c r="G3" s="199"/>
-      <c r="H3" s="199"/>
-      <c r="I3" s="199"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
+      <c r="F3" s="181"/>
+      <c r="G3" s="181"/>
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
     </row>
     <row r="4" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="199" t="s">
+      <c r="A4" s="181" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="199"/>
-      <c r="C4" s="199"/>
-      <c r="D4" s="199"/>
-      <c r="E4" s="199"/>
-      <c r="F4" s="199"/>
-      <c r="G4" s="199"/>
-      <c r="H4" s="199"/>
-      <c r="I4" s="199"/>
+      <c r="B4" s="181"/>
+      <c r="C4" s="181"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="181"/>
+      <c r="F4" s="181"/>
+      <c r="G4" s="181"/>
+      <c r="H4" s="181"/>
+      <c r="I4" s="181"/>
     </row>
     <row r="5" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="199" t="s">
+      <c r="A5" s="181" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="199"/>
-      <c r="C5" s="199"/>
-      <c r="D5" s="199"/>
-      <c r="E5" s="199"/>
-      <c r="F5" s="199"/>
-      <c r="G5" s="199"/>
-      <c r="H5" s="199"/>
-      <c r="I5" s="199"/>
+      <c r="B5" s="181"/>
+      <c r="C5" s="181"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
     </row>
     <row r="6" spans="1:9" s="9" customFormat="1" ht="7.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="190"/>
-      <c r="D6" s="190"/>
-      <c r="E6" s="190"/>
-      <c r="F6" s="190"/>
-      <c r="G6" s="190"/>
-      <c r="H6" s="190"/>
-      <c r="I6" s="190"/>
+      <c r="C6" s="183"/>
+      <c r="D6" s="183"/>
+      <c r="E6" s="183"/>
+      <c r="F6" s="183"/>
+      <c r="G6" s="183"/>
+      <c r="H6" s="183"/>
+      <c r="I6" s="183"/>
     </row>
     <row r="7" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="str">
         <f>'PC 1'!A1</f>
         <v xml:space="preserve">Particulars of Contract: </v>
       </c>
-      <c r="C7" s="190"/>
-      <c r="D7" s="190"/>
-      <c r="E7" s="190"/>
-      <c r="F7" s="190"/>
-      <c r="G7" s="190"/>
-      <c r="H7" s="190"/>
-      <c r="I7" s="190"/>
+      <c r="C7" s="183"/>
+      <c r="D7" s="183"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="183"/>
+      <c r="G7" s="183"/>
+      <c r="H7" s="183"/>
+      <c r="I7" s="183"/>
     </row>
     <row r="8" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="11" t="s">
@@ -7626,16 +7116,16 @@
       <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="192">
+      <c r="C8" s="182">
         <f>'PC 1'!B20</f>
         <v>0</v>
       </c>
-      <c r="D8" s="192"/>
-      <c r="E8" s="192"/>
-      <c r="F8" s="192"/>
-      <c r="G8" s="192"/>
-      <c r="H8" s="192"/>
-      <c r="I8" s="192"/>
+      <c r="D8" s="182"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="182"/>
+      <c r="H8" s="182"/>
+      <c r="I8" s="182"/>
     </row>
     <row r="9" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="11" t="s">
@@ -7644,16 +7134,16 @@
       <c r="B9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="193">
+      <c r="C9" s="179">
         <f>'PC 1'!B21</f>
         <v>0</v>
       </c>
-      <c r="D9" s="193"/>
-      <c r="E9" s="193"/>
-      <c r="F9" s="193"/>
-      <c r="G9" s="193"/>
-      <c r="H9" s="193"/>
-      <c r="I9" s="193"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="179"/>
+      <c r="H9" s="179"/>
+      <c r="I9" s="179"/>
     </row>
     <row r="10" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
@@ -7662,16 +7152,16 @@
       <c r="B10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="193">
+      <c r="C10" s="179">
         <f>'PC 1'!B22</f>
         <v>0</v>
       </c>
-      <c r="D10" s="193"/>
-      <c r="E10" s="193"/>
-      <c r="F10" s="193"/>
-      <c r="G10" s="193"/>
-      <c r="H10" s="193"/>
-      <c r="I10" s="193"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="179"/>
+      <c r="F10" s="179"/>
+      <c r="G10" s="179"/>
+      <c r="H10" s="179"/>
+      <c r="I10" s="179"/>
     </row>
     <row r="11" spans="1:9" s="9" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="11" t="s">
@@ -7680,16 +7170,16 @@
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="200">
+      <c r="C11" s="184">
         <f>'PC 1'!B23</f>
         <v>0</v>
       </c>
-      <c r="D11" s="200"/>
-      <c r="E11" s="200"/>
-      <c r="F11" s="200"/>
-      <c r="G11" s="200"/>
-      <c r="H11" s="200"/>
-      <c r="I11" s="200"/>
+      <c r="D11" s="184"/>
+      <c r="E11" s="184"/>
+      <c r="F11" s="184"/>
+      <c r="G11" s="184"/>
+      <c r="H11" s="184"/>
+      <c r="I11" s="184"/>
     </row>
     <row r="12" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="11" t="s">
@@ -7698,16 +7188,16 @@
       <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="193">
+      <c r="C12" s="179">
         <f>'PC 1'!B26</f>
         <v>0</v>
       </c>
-      <c r="D12" s="193"/>
-      <c r="E12" s="193"/>
-      <c r="F12" s="193"/>
-      <c r="G12" s="193"/>
-      <c r="H12" s="193"/>
-      <c r="I12" s="193"/>
+      <c r="D12" s="179"/>
+      <c r="E12" s="179"/>
+      <c r="F12" s="179"/>
+      <c r="G12" s="179"/>
+      <c r="H12" s="179"/>
+      <c r="I12" s="179"/>
     </row>
     <row r="13" spans="1:9" s="9" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="11" t="s">
@@ -7716,16 +7206,16 @@
       <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="193">
+      <c r="C13" s="179">
         <f>'PC 1'!B27</f>
         <v>0</v>
       </c>
-      <c r="D13" s="193"/>
-      <c r="E13" s="193"/>
-      <c r="F13" s="193"/>
-      <c r="G13" s="193"/>
-      <c r="H13" s="193"/>
-      <c r="I13" s="193"/>
+      <c r="D13" s="179"/>
+      <c r="E13" s="179"/>
+      <c r="F13" s="179"/>
+      <c r="G13" s="179"/>
+      <c r="H13" s="179"/>
+      <c r="I13" s="179"/>
     </row>
     <row r="14" spans="1:9" s="9" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="11" t="s">
@@ -7734,16 +7224,16 @@
       <c r="B14" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C14" s="193">
+      <c r="C14" s="179">
         <f>'PC 1'!D27</f>
         <v>0</v>
       </c>
-      <c r="D14" s="193"/>
-      <c r="E14" s="193"/>
-      <c r="F14" s="193"/>
-      <c r="G14" s="193"/>
-      <c r="H14" s="193"/>
-      <c r="I14" s="193"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="179"/>
+      <c r="F14" s="179"/>
+      <c r="G14" s="179"/>
+      <c r="H14" s="179"/>
+      <c r="I14" s="179"/>
     </row>
     <row r="15" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="11" t="s">
@@ -7752,16 +7242,16 @@
       <c r="B15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="193">
+      <c r="C15" s="179">
         <f>'PC 1'!B29</f>
         <v>0</v>
       </c>
-      <c r="D15" s="193"/>
-      <c r="E15" s="193"/>
-      <c r="F15" s="193"/>
-      <c r="G15" s="193"/>
-      <c r="H15" s="193"/>
-      <c r="I15" s="193"/>
+      <c r="D15" s="179"/>
+      <c r="E15" s="179"/>
+      <c r="F15" s="179"/>
+      <c r="G15" s="179"/>
+      <c r="H15" s="179"/>
+      <c r="I15" s="179"/>
     </row>
     <row r="16" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="11" t="s">
@@ -7770,16 +7260,16 @@
       <c r="B16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="193">
+      <c r="C16" s="179">
         <f>'PC 1'!B31</f>
         <v>0</v>
       </c>
-      <c r="D16" s="193"/>
-      <c r="E16" s="193"/>
-      <c r="F16" s="193"/>
-      <c r="G16" s="193"/>
-      <c r="H16" s="193"/>
-      <c r="I16" s="193"/>
+      <c r="D16" s="179"/>
+      <c r="E16" s="179"/>
+      <c r="F16" s="179"/>
+      <c r="G16" s="179"/>
+      <c r="H16" s="179"/>
+      <c r="I16" s="179"/>
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="11" t="s">
@@ -7788,16 +7278,16 @@
       <c r="B17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="193">
+      <c r="C17" s="179">
         <f>'PC 1'!B32</f>
         <v>0</v>
       </c>
-      <c r="D17" s="193"/>
-      <c r="E17" s="193"/>
-      <c r="F17" s="193"/>
-      <c r="G17" s="193"/>
-      <c r="H17" s="193"/>
-      <c r="I17" s="193"/>
+      <c r="D17" s="179"/>
+      <c r="E17" s="179"/>
+      <c r="F17" s="179"/>
+      <c r="G17" s="179"/>
+      <c r="H17" s="179"/>
+      <c r="I17" s="179"/>
     </row>
     <row r="18" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="11" t="s">
@@ -7806,16 +7296,16 @@
       <c r="B18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="193">
+      <c r="C18" s="179">
         <f>'PC 1'!B33</f>
         <v>0</v>
       </c>
-      <c r="D18" s="193"/>
-      <c r="E18" s="193"/>
-      <c r="F18" s="193"/>
-      <c r="G18" s="193"/>
-      <c r="H18" s="193"/>
-      <c r="I18" s="193"/>
+      <c r="D18" s="179"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="179"/>
+      <c r="G18" s="179"/>
+      <c r="H18" s="179"/>
+      <c r="I18" s="179"/>
     </row>
     <row r="19" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="11" t="s">
@@ -7914,16 +7404,16 @@
       <c r="B24" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="191">
+      <c r="C24" s="193">
         <f>'PC 1'!B34</f>
         <v>0</v>
       </c>
-      <c r="D24" s="192"/>
-      <c r="E24" s="192"/>
-      <c r="F24" s="192"/>
-      <c r="G24" s="192"/>
-      <c r="H24" s="192"/>
-      <c r="I24" s="192"/>
+      <c r="D24" s="182"/>
+      <c r="E24" s="182"/>
+      <c r="F24" s="182"/>
+      <c r="G24" s="182"/>
+      <c r="H24" s="182"/>
+      <c r="I24" s="182"/>
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="11" t="s">
@@ -7932,16 +7422,16 @@
       <c r="B25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="193">
+      <c r="C25" s="179">
         <f>'PC 1'!B35</f>
         <v>0</v>
       </c>
-      <c r="D25" s="193"/>
-      <c r="E25" s="193"/>
-      <c r="F25" s="193"/>
-      <c r="G25" s="193"/>
-      <c r="H25" s="193"/>
-      <c r="I25" s="193"/>
+      <c r="D25" s="179"/>
+      <c r="E25" s="179"/>
+      <c r="F25" s="179"/>
+      <c r="G25" s="179"/>
+      <c r="H25" s="179"/>
+      <c r="I25" s="179"/>
     </row>
     <row r="26" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="11" t="s">
@@ -8004,39 +7494,39 @@
       <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="193" t="s">
+      <c r="C29" s="179" t="s">
         <v>103</v>
       </c>
-      <c r="D29" s="193"/>
-      <c r="E29" s="193"/>
-      <c r="F29" s="193"/>
-      <c r="G29" s="193"/>
-      <c r="H29" s="193"/>
-      <c r="I29" s="193"/>
+      <c r="D29" s="179"/>
+      <c r="E29" s="179"/>
+      <c r="F29" s="179"/>
+      <c r="G29" s="179"/>
+      <c r="H29" s="179"/>
+      <c r="I29" s="179"/>
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="11"/>
       <c r="B30" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="193"/>
-      <c r="D30" s="193"/>
-      <c r="E30" s="193"/>
-      <c r="F30" s="193"/>
-      <c r="G30" s="193"/>
-      <c r="H30" s="193"/>
-      <c r="I30" s="193"/>
+      <c r="C30" s="179"/>
+      <c r="D30" s="179"/>
+      <c r="E30" s="179"/>
+      <c r="F30" s="179"/>
+      <c r="G30" s="179"/>
+      <c r="H30" s="179"/>
+      <c r="I30" s="179"/>
     </row>
     <row r="31" spans="1:9" s="9" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="190"/>
-      <c r="B31" s="190"/>
-      <c r="C31" s="190"/>
-      <c r="D31" s="190"/>
-      <c r="E31" s="190"/>
-      <c r="F31" s="190"/>
-      <c r="G31" s="190"/>
-      <c r="H31" s="190"/>
-      <c r="I31" s="190"/>
+      <c r="A31" s="183"/>
+      <c r="B31" s="183"/>
+      <c r="C31" s="183"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="183"/>
+      <c r="F31" s="183"/>
+      <c r="G31" s="183"/>
+      <c r="H31" s="183"/>
+      <c r="I31" s="183"/>
     </row>
     <row r="32" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A32" s="189" t="s">
@@ -8055,61 +7545,61 @@
       <c r="A33" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="190" t="s">
+      <c r="B33" s="183" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="190"/>
-      <c r="D33" s="190"/>
-      <c r="E33" s="190"/>
-      <c r="F33" s="190"/>
-      <c r="G33" s="190"/>
-      <c r="H33" s="190"/>
-      <c r="I33" s="190"/>
+      <c r="C33" s="183"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="183"/>
+      <c r="F33" s="183"/>
+      <c r="G33" s="183"/>
+      <c r="H33" s="183"/>
+      <c r="I33" s="183"/>
     </row>
     <row r="34" spans="1:10" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A34" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="190" t="s">
+      <c r="B34" s="183" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="190"/>
-      <c r="D34" s="190"/>
-      <c r="E34" s="190"/>
-      <c r="F34" s="190"/>
-      <c r="G34" s="190"/>
-      <c r="H34" s="190"/>
-      <c r="I34" s="190"/>
+      <c r="C34" s="183"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="183"/>
+      <c r="F34" s="183"/>
+      <c r="G34" s="183"/>
+      <c r="H34" s="183"/>
+      <c r="I34" s="183"/>
     </row>
     <row r="35" spans="1:10" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A35" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="190" t="s">
+      <c r="B35" s="183" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="190"/>
-      <c r="D35" s="190"/>
-      <c r="E35" s="190"/>
-      <c r="F35" s="190"/>
-      <c r="G35" s="190"/>
-      <c r="H35" s="190"/>
-      <c r="I35" s="190"/>
+      <c r="C35" s="183"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="183"/>
+      <c r="F35" s="183"/>
+      <c r="G35" s="183"/>
+      <c r="H35" s="183"/>
+      <c r="I35" s="183"/>
     </row>
     <row r="36" spans="1:10" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A36" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="190" t="s">
+      <c r="B36" s="183" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="190"/>
-      <c r="D36" s="190"/>
-      <c r="E36" s="190"/>
-      <c r="F36" s="190"/>
-      <c r="G36" s="190"/>
-      <c r="H36" s="190"/>
-      <c r="I36" s="190"/>
+      <c r="C36" s="183"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="183"/>
+      <c r="F36" s="183"/>
+      <c r="G36" s="183"/>
+      <c r="H36" s="183"/>
+      <c r="I36" s="183"/>
     </row>
     <row r="37" spans="1:10" s="9" customFormat="1" ht="22.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="189" t="s">
@@ -8125,255 +7615,215 @@
       <c r="I37" s="189"/>
     </row>
     <row r="38" spans="1:10" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="195" t="str">
+      <c r="A38" s="186" t="str">
         <f>'PC 1'!A16</f>
         <v>Certification of the sum of ₦0.00 () only, in favour of 0 is recommended, please.</v>
       </c>
-      <c r="B38" s="195"/>
-      <c r="C38" s="195"/>
-      <c r="D38" s="195"/>
-      <c r="E38" s="195"/>
-      <c r="F38" s="195"/>
-      <c r="G38" s="195"/>
-      <c r="H38" s="195"/>
-      <c r="I38" s="195"/>
+      <c r="B38" s="186"/>
+      <c r="C38" s="186"/>
+      <c r="D38" s="186"/>
+      <c r="E38" s="186"/>
+      <c r="F38" s="186"/>
+      <c r="G38" s="186"/>
+      <c r="H38" s="186"/>
+      <c r="I38" s="186"/>
     </row>
     <row r="39" spans="1:10" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A39" s="195"/>
-      <c r="B39" s="195"/>
-      <c r="C39" s="195"/>
-      <c r="D39" s="195"/>
-      <c r="E39" s="195"/>
-      <c r="F39" s="195"/>
-      <c r="G39" s="195"/>
-      <c r="H39" s="195"/>
-      <c r="I39" s="195"/>
+      <c r="A39" s="186"/>
+      <c r="B39" s="186"/>
+      <c r="C39" s="186"/>
+      <c r="D39" s="186"/>
+      <c r="E39" s="186"/>
+      <c r="F39" s="186"/>
+      <c r="G39" s="186"/>
+      <c r="H39" s="186"/>
+      <c r="I39" s="186"/>
     </row>
     <row r="40" spans="1:10" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A40" s="195"/>
-      <c r="B40" s="195"/>
-      <c r="C40" s="195"/>
-      <c r="D40" s="195"/>
-      <c r="E40" s="195"/>
-      <c r="F40" s="195"/>
-      <c r="G40" s="195"/>
-      <c r="H40" s="195"/>
-      <c r="I40" s="195"/>
+      <c r="A40" s="186"/>
+      <c r="B40" s="186"/>
+      <c r="C40" s="186"/>
+      <c r="D40" s="186"/>
+      <c r="E40" s="186"/>
+      <c r="F40" s="186"/>
+      <c r="G40" s="186"/>
+      <c r="H40" s="186"/>
+      <c r="I40" s="186"/>
     </row>
     <row r="41" spans="1:10" s="9" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="198"/>
-      <c r="B41" s="198"/>
-      <c r="C41" s="198"/>
-      <c r="D41" s="198"/>
-      <c r="E41" s="198"/>
-      <c r="F41" s="198"/>
-      <c r="G41" s="198"/>
-      <c r="H41" s="198"/>
-      <c r="I41" s="198"/>
+      <c r="A41" s="190"/>
+      <c r="B41" s="190"/>
+      <c r="C41" s="190"/>
+      <c r="D41" s="190"/>
+      <c r="E41" s="190"/>
+      <c r="F41" s="190"/>
+      <c r="G41" s="190"/>
+      <c r="H41" s="190"/>
+      <c r="I41" s="190"/>
     </row>
     <row r="42" spans="1:10" s="9" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="198"/>
-      <c r="B42" s="198"/>
-      <c r="C42" s="198"/>
-      <c r="D42" s="198"/>
-      <c r="E42" s="198"/>
-      <c r="F42" s="198"/>
-      <c r="G42" s="198"/>
-      <c r="H42" s="198"/>
-      <c r="I42" s="198"/>
+      <c r="A42" s="190"/>
+      <c r="B42" s="190"/>
+      <c r="C42" s="190"/>
+      <c r="D42" s="190"/>
+      <c r="E42" s="190"/>
+      <c r="F42" s="190"/>
+      <c r="G42" s="190"/>
+      <c r="H42" s="190"/>
+      <c r="I42" s="190"/>
     </row>
     <row r="43" spans="1:10" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="183" t="s">
+      <c r="A43" s="191" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="184"/>
-      <c r="C43" s="184"/>
-      <c r="D43" s="197" t="s">
+      <c r="B43" s="192"/>
+      <c r="C43" s="192"/>
+      <c r="D43" s="188" t="s">
         <v>53</v>
       </c>
-      <c r="E43" s="197"/>
-      <c r="F43" s="197"/>
-      <c r="G43" s="197"/>
-      <c r="H43" s="197"/>
-      <c r="I43" s="197"/>
+      <c r="E43" s="188"/>
+      <c r="F43" s="188"/>
+      <c r="G43" s="188"/>
+      <c r="H43" s="188"/>
+      <c r="I43" s="188"/>
     </row>
     <row r="44" spans="1:10" s="9" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="196" t="s">
+      <c r="A44" s="187" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="196"/>
-      <c r="C44" s="196"/>
-      <c r="D44" s="194" t="str">
+      <c r="B44" s="187"/>
+      <c r="C44" s="187"/>
+      <c r="D44" s="185" t="str">
         <f>'PC 1'!B68</f>
         <v>Alawiye, K.T (Ms)</v>
       </c>
-      <c r="E44" s="194"/>
-      <c r="F44" s="194"/>
-      <c r="G44" s="194"/>
-      <c r="H44" s="194"/>
-      <c r="I44" s="194"/>
+      <c r="E44" s="185"/>
+      <c r="F44" s="185"/>
+      <c r="G44" s="185"/>
+      <c r="H44" s="185"/>
+      <c r="I44" s="185"/>
     </row>
     <row r="45" spans="1:10" s="9" customFormat="1" ht="22.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="196" t="s">
+      <c r="A45" s="187" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="196"/>
-      <c r="C45" s="196"/>
-      <c r="D45" s="194" t="str">
+      <c r="B45" s="187"/>
+      <c r="C45" s="187"/>
+      <c r="D45" s="185" t="str">
         <f>'PC 1'!B69</f>
         <v>PPO (MED)</v>
       </c>
-      <c r="E45" s="194"/>
-      <c r="F45" s="194"/>
-      <c r="G45" s="194"/>
-      <c r="H45" s="194"/>
-      <c r="I45" s="194"/>
+      <c r="E45" s="185"/>
+      <c r="F45" s="185"/>
+      <c r="G45" s="185"/>
+      <c r="H45" s="185"/>
+      <c r="I45" s="185"/>
     </row>
     <row r="46" spans="1:10" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="181"/>
-      <c r="B46" s="181"/>
-      <c r="C46" s="181"/>
-      <c r="D46" s="186">
+      <c r="A46" s="196"/>
+      <c r="B46" s="196"/>
+      <c r="C46" s="196"/>
+      <c r="D46" s="199">
         <f>'PC 1'!B36</f>
         <v>0</v>
       </c>
-      <c r="E46" s="186"/>
-      <c r="F46" s="186"/>
-      <c r="G46" s="186"/>
-      <c r="H46" s="186"/>
-      <c r="I46" s="186"/>
+      <c r="E46" s="199"/>
+      <c r="F46" s="199"/>
+      <c r="G46" s="199"/>
+      <c r="H46" s="199"/>
+      <c r="I46" s="199"/>
       <c r="J46" s="12"/>
     </row>
     <row r="47" spans="1:10" s="9" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="182" t="s">
+      <c r="A47" s="197" t="s">
         <v>55</v>
       </c>
-      <c r="B47" s="182"/>
-      <c r="C47" s="182"/>
-      <c r="D47" s="182"/>
-      <c r="E47" s="182"/>
-      <c r="F47" s="182"/>
-      <c r="G47" s="182"/>
-      <c r="H47" s="182"/>
+      <c r="B47" s="197"/>
+      <c r="C47" s="197"/>
+      <c r="D47" s="197"/>
+      <c r="E47" s="197"/>
+      <c r="F47" s="197"/>
+      <c r="G47" s="197"/>
+      <c r="H47" s="197"/>
     </row>
     <row r="48" spans="1:10" s="9" customFormat="1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="182"/>
-      <c r="B48" s="182"/>
-      <c r="C48" s="182"/>
-      <c r="D48" s="182"/>
-      <c r="E48" s="182"/>
-      <c r="F48" s="182"/>
-      <c r="G48" s="182"/>
-      <c r="H48" s="182"/>
+      <c r="A48" s="197"/>
+      <c r="B48" s="197"/>
+      <c r="C48" s="197"/>
+      <c r="D48" s="197"/>
+      <c r="E48" s="197"/>
+      <c r="F48" s="197"/>
+      <c r="G48" s="197"/>
+      <c r="H48" s="197"/>
     </row>
     <row r="49" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="182"/>
-      <c r="B49" s="182"/>
-      <c r="C49" s="182"/>
-      <c r="D49" s="182"/>
-      <c r="E49" s="182"/>
-      <c r="F49" s="182"/>
-      <c r="G49" s="182"/>
-      <c r="H49" s="182"/>
+      <c r="A49" s="197"/>
+      <c r="B49" s="197"/>
+      <c r="C49" s="197"/>
+      <c r="D49" s="197"/>
+      <c r="E49" s="197"/>
+      <c r="F49" s="197"/>
+      <c r="G49" s="197"/>
+      <c r="H49" s="197"/>
     </row>
     <row r="50" spans="1:9" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="183" t="s">
+      <c r="A50" s="191" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="184"/>
-      <c r="C50" s="185" t="s">
+      <c r="B50" s="192"/>
+      <c r="C50" s="198" t="s">
         <v>100</v>
       </c>
-      <c r="D50" s="182"/>
-      <c r="E50" s="187" t="s">
+      <c r="D50" s="197"/>
+      <c r="E50" s="200" t="s">
         <v>100</v>
       </c>
-      <c r="F50" s="187"/>
-      <c r="G50" s="187"/>
-      <c r="H50" s="187"/>
-      <c r="I50" s="187"/>
+      <c r="F50" s="200"/>
+      <c r="G50" s="200"/>
+      <c r="H50" s="200"/>
+      <c r="I50" s="200"/>
     </row>
     <row r="51" spans="1:9" s="10" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="179" t="s">
+      <c r="A51" s="194" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="179"/>
-      <c r="C51" s="180" t="s">
+      <c r="B51" s="194"/>
+      <c r="C51" s="195" t="s">
         <v>96</v>
       </c>
-      <c r="D51" s="180"/>
-      <c r="E51" s="188" t="s">
+      <c r="D51" s="195"/>
+      <c r="E51" s="180" t="s">
         <v>97</v>
       </c>
-      <c r="F51" s="188"/>
-      <c r="G51" s="188"/>
-      <c r="H51" s="188"/>
-      <c r="I51" s="188"/>
+      <c r="F51" s="180"/>
+      <c r="G51" s="180"/>
+      <c r="H51" s="180"/>
+      <c r="I51" s="180"/>
     </row>
     <row r="52" spans="1:9" s="10" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="179" t="s">
+      <c r="A52" s="194" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="179"/>
-      <c r="C52" s="180" t="s">
+      <c r="B52" s="194"/>
+      <c r="C52" s="195" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="180"/>
-      <c r="E52" s="188" t="s">
+      <c r="D52" s="195"/>
+      <c r="E52" s="180" t="s">
         <v>101</v>
       </c>
-      <c r="F52" s="188"/>
-      <c r="G52" s="188"/>
-      <c r="H52" s="188"/>
-      <c r="I52" s="188"/>
+      <c r="F52" s="180"/>
+      <c r="G52" s="180"/>
+      <c r="H52" s="180"/>
+      <c r="I52" s="180"/>
     </row>
     <row r="53" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="54" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="55" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="T45iWvNsr1hGkYSAl60cPBBGEmTqPHx7n0KlTBgAQMIMqWHejcg1l6z16ijGNlfOp0B0e97qSW8giO8aPp12sA==" saltValue="ZO+Z89g6yR6WPkMr+p99cw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="H9zoclxu4UsZj8+rBjW9H22erWzDUi501CBH4rrWuTPFpEO4+iRDcmY3jDBt0t9RxswI7OWiDBBTMio5T4W7Tw==" saltValue="NaHk3uBWzHvDeSenCoPVOg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="56">
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C15:I15"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="C17:I17"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="C19:I19"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="D45:I45"/>
-    <mergeCell ref="A38:I40"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D43:I43"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B36:I36"/>
-    <mergeCell ref="A37:I37"/>
-    <mergeCell ref="A41:I42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:I44"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="C22:I22"/>
     <mergeCell ref="A52:B52"/>
@@ -8390,6 +7840,46 @@
     <mergeCell ref="E52:I52"/>
     <mergeCell ref="A32:I32"/>
     <mergeCell ref="B33:I33"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="D45:I45"/>
+    <mergeCell ref="A38:I40"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D43:I43"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="A37:I37"/>
+    <mergeCell ref="A41:I42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:I44"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="C17:I17"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="C19:I19"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8406,7 +7896,7 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A2" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C26" sqref="C26:I26"/>
     </sheetView>
   </sheetViews>
@@ -8429,79 +7919,79 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="188">
+      <c r="A2" s="180">
         <f>'PC 2'!B55</f>
         <v>0</v>
       </c>
-      <c r="B2" s="188"/>
-      <c r="C2" s="188"/>
-      <c r="D2" s="188"/>
-      <c r="E2" s="188"/>
-      <c r="F2" s="188"/>
-      <c r="G2" s="188"/>
-      <c r="H2" s="188"/>
-      <c r="I2" s="188"/>
+      <c r="B2" s="180"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
+      <c r="I2" s="180"/>
     </row>
     <row r="3" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="199" t="s">
+      <c r="A3" s="181" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="199"/>
-      <c r="C3" s="199"/>
-      <c r="D3" s="199"/>
-      <c r="E3" s="199"/>
-      <c r="F3" s="199"/>
-      <c r="G3" s="199"/>
-      <c r="H3" s="199"/>
-      <c r="I3" s="199"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
+      <c r="F3" s="181"/>
+      <c r="G3" s="181"/>
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
     </row>
     <row r="4" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="199" t="s">
+      <c r="A4" s="181" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="199"/>
-      <c r="C4" s="199"/>
-      <c r="D4" s="199"/>
-      <c r="E4" s="199"/>
-      <c r="F4" s="199"/>
-      <c r="G4" s="199"/>
-      <c r="H4" s="199"/>
-      <c r="I4" s="199"/>
+      <c r="B4" s="181"/>
+      <c r="C4" s="181"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="181"/>
+      <c r="F4" s="181"/>
+      <c r="G4" s="181"/>
+      <c r="H4" s="181"/>
+      <c r="I4" s="181"/>
     </row>
     <row r="5" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="199" t="s">
+      <c r="A5" s="181" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="199"/>
-      <c r="C5" s="199"/>
-      <c r="D5" s="199"/>
-      <c r="E5" s="199"/>
-      <c r="F5" s="199"/>
-      <c r="G5" s="199"/>
-      <c r="H5" s="199"/>
-      <c r="I5" s="199"/>
+      <c r="B5" s="181"/>
+      <c r="C5" s="181"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
     </row>
     <row r="6" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="C6" s="190"/>
-      <c r="D6" s="190"/>
-      <c r="E6" s="190"/>
-      <c r="F6" s="190"/>
-      <c r="G6" s="190"/>
-      <c r="H6" s="190"/>
-      <c r="I6" s="190"/>
+      <c r="C6" s="183"/>
+      <c r="D6" s="183"/>
+      <c r="E6" s="183"/>
+      <c r="F6" s="183"/>
+      <c r="G6" s="183"/>
+      <c r="H6" s="183"/>
+      <c r="I6" s="183"/>
     </row>
     <row r="7" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="str">
         <f>'PC 2'!A1</f>
         <v xml:space="preserve">Particulars of Contract: </v>
       </c>
-      <c r="C7" s="190"/>
-      <c r="D7" s="190"/>
-      <c r="E7" s="190"/>
-      <c r="F7" s="190"/>
-      <c r="G7" s="190"/>
-      <c r="H7" s="190"/>
-      <c r="I7" s="190"/>
+      <c r="C7" s="183"/>
+      <c r="D7" s="183"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="183"/>
+      <c r="G7" s="183"/>
+      <c r="H7" s="183"/>
+      <c r="I7" s="183"/>
     </row>
     <row r="8" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="11" t="s">
@@ -8510,16 +8000,16 @@
       <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="192">
+      <c r="C8" s="182">
         <f>'PC 2'!B20</f>
         <v>0</v>
       </c>
-      <c r="D8" s="192"/>
-      <c r="E8" s="192"/>
-      <c r="F8" s="192"/>
-      <c r="G8" s="192"/>
-      <c r="H8" s="192"/>
-      <c r="I8" s="192"/>
+      <c r="D8" s="182"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="182"/>
+      <c r="H8" s="182"/>
+      <c r="I8" s="182"/>
     </row>
     <row r="9" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="11" t="s">
@@ -8528,16 +8018,16 @@
       <c r="B9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="193">
+      <c r="C9" s="179">
         <f>'PC 2'!B21</f>
         <v>0</v>
       </c>
-      <c r="D9" s="193"/>
-      <c r="E9" s="193"/>
-      <c r="F9" s="193"/>
-      <c r="G9" s="193"/>
-      <c r="H9" s="193"/>
-      <c r="I9" s="193"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="179"/>
+      <c r="H9" s="179"/>
+      <c r="I9" s="179"/>
     </row>
     <row r="10" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
@@ -8546,16 +8036,16 @@
       <c r="B10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="193">
+      <c r="C10" s="179">
         <f>'PC 2'!B22</f>
         <v>0</v>
       </c>
-      <c r="D10" s="193"/>
-      <c r="E10" s="193"/>
-      <c r="F10" s="193"/>
-      <c r="G10" s="193"/>
-      <c r="H10" s="193"/>
-      <c r="I10" s="193"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="179"/>
+      <c r="F10" s="179"/>
+      <c r="G10" s="179"/>
+      <c r="H10" s="179"/>
+      <c r="I10" s="179"/>
     </row>
     <row r="11" spans="1:9" s="9" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="11" t="s">
@@ -8564,16 +8054,16 @@
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="200">
+      <c r="C11" s="184">
         <f>'PC 2'!B23</f>
         <v>0</v>
       </c>
-      <c r="D11" s="200"/>
-      <c r="E11" s="200"/>
-      <c r="F11" s="200"/>
-      <c r="G11" s="200"/>
-      <c r="H11" s="200"/>
-      <c r="I11" s="200"/>
+      <c r="D11" s="184"/>
+      <c r="E11" s="184"/>
+      <c r="F11" s="184"/>
+      <c r="G11" s="184"/>
+      <c r="H11" s="184"/>
+      <c r="I11" s="184"/>
     </row>
     <row r="12" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="11" t="s">
@@ -8582,16 +8072,16 @@
       <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="193">
+      <c r="C12" s="179">
         <f>'PC 2'!B26</f>
         <v>0</v>
       </c>
-      <c r="D12" s="193"/>
-      <c r="E12" s="193"/>
-      <c r="F12" s="193"/>
-      <c r="G12" s="193"/>
-      <c r="H12" s="193"/>
-      <c r="I12" s="193"/>
+      <c r="D12" s="179"/>
+      <c r="E12" s="179"/>
+      <c r="F12" s="179"/>
+      <c r="G12" s="179"/>
+      <c r="H12" s="179"/>
+      <c r="I12" s="179"/>
     </row>
     <row r="13" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="11" t="s">
@@ -8600,16 +8090,16 @@
       <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="193">
+      <c r="C13" s="179">
         <f>'PC 2'!B27</f>
         <v>0</v>
       </c>
-      <c r="D13" s="193"/>
-      <c r="E13" s="193"/>
-      <c r="F13" s="193"/>
-      <c r="G13" s="193"/>
-      <c r="H13" s="193"/>
-      <c r="I13" s="193"/>
+      <c r="D13" s="179"/>
+      <c r="E13" s="179"/>
+      <c r="F13" s="179"/>
+      <c r="G13" s="179"/>
+      <c r="H13" s="179"/>
+      <c r="I13" s="179"/>
     </row>
     <row r="14" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="11" t="s">
@@ -8618,16 +8108,16 @@
       <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="193">
+      <c r="C14" s="179">
         <f>'PC 2'!D27</f>
         <v>0</v>
       </c>
-      <c r="D14" s="193"/>
-      <c r="E14" s="193"/>
-      <c r="F14" s="193"/>
-      <c r="G14" s="193"/>
-      <c r="H14" s="193"/>
-      <c r="I14" s="193"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="179"/>
+      <c r="F14" s="179"/>
+      <c r="G14" s="179"/>
+      <c r="H14" s="179"/>
+      <c r="I14" s="179"/>
     </row>
     <row r="15" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="11" t="s">
@@ -8636,16 +8126,16 @@
       <c r="B15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="193">
+      <c r="C15" s="179">
         <f>'PC 2'!B29</f>
         <v>0</v>
       </c>
-      <c r="D15" s="193"/>
-      <c r="E15" s="193"/>
-      <c r="F15" s="193"/>
-      <c r="G15" s="193"/>
-      <c r="H15" s="193"/>
-      <c r="I15" s="193"/>
+      <c r="D15" s="179"/>
+      <c r="E15" s="179"/>
+      <c r="F15" s="179"/>
+      <c r="G15" s="179"/>
+      <c r="H15" s="179"/>
+      <c r="I15" s="179"/>
     </row>
     <row r="16" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="11" t="s">
@@ -8654,16 +8144,16 @@
       <c r="B16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="193">
+      <c r="C16" s="179">
         <f>'PC 2'!B31</f>
         <v>0</v>
       </c>
-      <c r="D16" s="193"/>
-      <c r="E16" s="193"/>
-      <c r="F16" s="193"/>
-      <c r="G16" s="193"/>
-      <c r="H16" s="193"/>
-      <c r="I16" s="193"/>
+      <c r="D16" s="179"/>
+      <c r="E16" s="179"/>
+      <c r="F16" s="179"/>
+      <c r="G16" s="179"/>
+      <c r="H16" s="179"/>
+      <c r="I16" s="179"/>
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="11" t="s">
@@ -8672,16 +8162,16 @@
       <c r="B17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="193">
+      <c r="C17" s="179">
         <f>'PC 2'!B32</f>
         <v>0</v>
       </c>
-      <c r="D17" s="193"/>
-      <c r="E17" s="193"/>
-      <c r="F17" s="193"/>
-      <c r="G17" s="193"/>
-      <c r="H17" s="193"/>
-      <c r="I17" s="193"/>
+      <c r="D17" s="179"/>
+      <c r="E17" s="179"/>
+      <c r="F17" s="179"/>
+      <c r="G17" s="179"/>
+      <c r="H17" s="179"/>
+      <c r="I17" s="179"/>
     </row>
     <row r="18" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="11" t="s">
@@ -8690,16 +8180,16 @@
       <c r="B18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="193">
+      <c r="C18" s="179">
         <f>'PC 2'!B33</f>
         <v>0</v>
       </c>
-      <c r="D18" s="193"/>
-      <c r="E18" s="193"/>
-      <c r="F18" s="193"/>
-      <c r="G18" s="193"/>
-      <c r="H18" s="193"/>
-      <c r="I18" s="193"/>
+      <c r="D18" s="179"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="179"/>
+      <c r="G18" s="179"/>
+      <c r="H18" s="179"/>
+      <c r="I18" s="179"/>
     </row>
     <row r="19" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="11" t="s">
@@ -8798,16 +8288,16 @@
       <c r="B24" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="191">
+      <c r="C24" s="193">
         <f>'PC 2'!B34</f>
         <v>0</v>
       </c>
-      <c r="D24" s="192"/>
-      <c r="E24" s="192"/>
-      <c r="F24" s="192"/>
-      <c r="G24" s="192"/>
-      <c r="H24" s="192"/>
-      <c r="I24" s="192"/>
+      <c r="D24" s="182"/>
+      <c r="E24" s="182"/>
+      <c r="F24" s="182"/>
+      <c r="G24" s="182"/>
+      <c r="H24" s="182"/>
+      <c r="I24" s="182"/>
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="11" t="s">
@@ -8816,16 +8306,16 @@
       <c r="B25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="193">
+      <c r="C25" s="179">
         <f>'PC 2'!B35</f>
         <v>0</v>
       </c>
-      <c r="D25" s="193"/>
-      <c r="E25" s="193"/>
-      <c r="F25" s="193"/>
-      <c r="G25" s="193"/>
-      <c r="H25" s="193"/>
-      <c r="I25" s="193"/>
+      <c r="D25" s="179"/>
+      <c r="E25" s="179"/>
+      <c r="F25" s="179"/>
+      <c r="G25" s="179"/>
+      <c r="H25" s="179"/>
+      <c r="I25" s="179"/>
     </row>
     <row r="26" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="11" t="s">
@@ -8888,39 +8378,39 @@
       <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="193" t="s">
+      <c r="C29" s="179" t="s">
         <v>103</v>
       </c>
-      <c r="D29" s="193"/>
-      <c r="E29" s="193"/>
-      <c r="F29" s="193"/>
-      <c r="G29" s="193"/>
-      <c r="H29" s="193"/>
-      <c r="I29" s="193"/>
+      <c r="D29" s="179"/>
+      <c r="E29" s="179"/>
+      <c r="F29" s="179"/>
+      <c r="G29" s="179"/>
+      <c r="H29" s="179"/>
+      <c r="I29" s="179"/>
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="11"/>
       <c r="B30" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="193"/>
-      <c r="D30" s="193"/>
-      <c r="E30" s="193"/>
-      <c r="F30" s="193"/>
-      <c r="G30" s="193"/>
-      <c r="H30" s="193"/>
-      <c r="I30" s="193"/>
+      <c r="C30" s="179"/>
+      <c r="D30" s="179"/>
+      <c r="E30" s="179"/>
+      <c r="F30" s="179"/>
+      <c r="G30" s="179"/>
+      <c r="H30" s="179"/>
+      <c r="I30" s="179"/>
     </row>
     <row r="31" spans="1:9" s="9" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="190"/>
-      <c r="B31" s="190"/>
-      <c r="C31" s="190"/>
-      <c r="D31" s="190"/>
-      <c r="E31" s="190"/>
-      <c r="F31" s="190"/>
-      <c r="G31" s="190"/>
-      <c r="H31" s="190"/>
-      <c r="I31" s="190"/>
+      <c r="A31" s="183"/>
+      <c r="B31" s="183"/>
+      <c r="C31" s="183"/>
+      <c r="D31" s="183"/>
+      <c r="E31" s="183"/>
+      <c r="F31" s="183"/>
+      <c r="G31" s="183"/>
+      <c r="H31" s="183"/>
+      <c r="I31" s="183"/>
     </row>
     <row r="32" spans="1:9" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A32" s="189" t="s">
@@ -8939,61 +8429,61 @@
       <c r="A33" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="190" t="s">
+      <c r="B33" s="183" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="190"/>
-      <c r="D33" s="190"/>
-      <c r="E33" s="190"/>
-      <c r="F33" s="190"/>
-      <c r="G33" s="190"/>
-      <c r="H33" s="190"/>
-      <c r="I33" s="190"/>
+      <c r="C33" s="183"/>
+      <c r="D33" s="183"/>
+      <c r="E33" s="183"/>
+      <c r="F33" s="183"/>
+      <c r="G33" s="183"/>
+      <c r="H33" s="183"/>
+      <c r="I33" s="183"/>
     </row>
     <row r="34" spans="1:10" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A34" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="190" t="s">
+      <c r="B34" s="183" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="190"/>
-      <c r="D34" s="190"/>
-      <c r="E34" s="190"/>
-      <c r="F34" s="190"/>
-      <c r="G34" s="190"/>
-      <c r="H34" s="190"/>
-      <c r="I34" s="190"/>
+      <c r="C34" s="183"/>
+      <c r="D34" s="183"/>
+      <c r="E34" s="183"/>
+      <c r="F34" s="183"/>
+      <c r="G34" s="183"/>
+      <c r="H34" s="183"/>
+      <c r="I34" s="183"/>
     </row>
     <row r="35" spans="1:10" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A35" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="190" t="s">
+      <c r="B35" s="183" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="190"/>
-      <c r="D35" s="190"/>
-      <c r="E35" s="190"/>
-      <c r="F35" s="190"/>
-      <c r="G35" s="190"/>
-      <c r="H35" s="190"/>
-      <c r="I35" s="190"/>
+      <c r="C35" s="183"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="183"/>
+      <c r="F35" s="183"/>
+      <c r="G35" s="183"/>
+      <c r="H35" s="183"/>
+      <c r="I35" s="183"/>
     </row>
     <row r="36" spans="1:10" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A36" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="190" t="s">
+      <c r="B36" s="183" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="190"/>
-      <c r="D36" s="190"/>
-      <c r="E36" s="190"/>
-      <c r="F36" s="190"/>
-      <c r="G36" s="190"/>
-      <c r="H36" s="190"/>
-      <c r="I36" s="190"/>
+      <c r="C36" s="183"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="183"/>
+      <c r="F36" s="183"/>
+      <c r="G36" s="183"/>
+      <c r="H36" s="183"/>
+      <c r="I36" s="183"/>
     </row>
     <row r="37" spans="1:10" s="9" customFormat="1" ht="22.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="189" t="s">
@@ -9009,203 +8499,243 @@
       <c r="I37" s="189"/>
     </row>
     <row r="38" spans="1:10" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="195" t="str">
+      <c r="A38" s="186" t="str">
         <f>'PC 2'!A16</f>
         <v>Certification of the sum of ₦0.00 () only, in favour of 0 is recommended, please.</v>
       </c>
-      <c r="B38" s="195"/>
-      <c r="C38" s="195"/>
-      <c r="D38" s="195"/>
-      <c r="E38" s="195"/>
-      <c r="F38" s="195"/>
-      <c r="G38" s="195"/>
-      <c r="H38" s="195"/>
-      <c r="I38" s="195"/>
+      <c r="B38" s="186"/>
+      <c r="C38" s="186"/>
+      <c r="D38" s="186"/>
+      <c r="E38" s="186"/>
+      <c r="F38" s="186"/>
+      <c r="G38" s="186"/>
+      <c r="H38" s="186"/>
+      <c r="I38" s="186"/>
     </row>
     <row r="39" spans="1:10" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A39" s="195"/>
-      <c r="B39" s="195"/>
-      <c r="C39" s="195"/>
-      <c r="D39" s="195"/>
-      <c r="E39" s="195"/>
-      <c r="F39" s="195"/>
-      <c r="G39" s="195"/>
-      <c r="H39" s="195"/>
-      <c r="I39" s="195"/>
+      <c r="A39" s="186"/>
+      <c r="B39" s="186"/>
+      <c r="C39" s="186"/>
+      <c r="D39" s="186"/>
+      <c r="E39" s="186"/>
+      <c r="F39" s="186"/>
+      <c r="G39" s="186"/>
+      <c r="H39" s="186"/>
+      <c r="I39" s="186"/>
     </row>
     <row r="40" spans="1:10" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A40" s="195"/>
-      <c r="B40" s="195"/>
-      <c r="C40" s="195"/>
-      <c r="D40" s="195"/>
-      <c r="E40" s="195"/>
-      <c r="F40" s="195"/>
-      <c r="G40" s="195"/>
-      <c r="H40" s="195"/>
-      <c r="I40" s="195"/>
+      <c r="A40" s="186"/>
+      <c r="B40" s="186"/>
+      <c r="C40" s="186"/>
+      <c r="D40" s="186"/>
+      <c r="E40" s="186"/>
+      <c r="F40" s="186"/>
+      <c r="G40" s="186"/>
+      <c r="H40" s="186"/>
+      <c r="I40" s="186"/>
     </row>
     <row r="41" spans="1:10" s="9" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="198"/>
-      <c r="B41" s="198"/>
-      <c r="C41" s="198"/>
-      <c r="D41" s="198"/>
-      <c r="E41" s="198"/>
-      <c r="F41" s="198"/>
-      <c r="G41" s="198"/>
-      <c r="H41" s="198"/>
-      <c r="I41" s="198"/>
+      <c r="A41" s="190"/>
+      <c r="B41" s="190"/>
+      <c r="C41" s="190"/>
+      <c r="D41" s="190"/>
+      <c r="E41" s="190"/>
+      <c r="F41" s="190"/>
+      <c r="G41" s="190"/>
+      <c r="H41" s="190"/>
+      <c r="I41" s="190"/>
     </row>
     <row r="42" spans="1:10" s="9" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="198"/>
-      <c r="B42" s="198"/>
-      <c r="C42" s="198"/>
-      <c r="D42" s="198"/>
-      <c r="E42" s="198"/>
-      <c r="F42" s="198"/>
-      <c r="G42" s="198"/>
-      <c r="H42" s="198"/>
-      <c r="I42" s="198"/>
+      <c r="A42" s="190"/>
+      <c r="B42" s="190"/>
+      <c r="C42" s="190"/>
+      <c r="D42" s="190"/>
+      <c r="E42" s="190"/>
+      <c r="F42" s="190"/>
+      <c r="G42" s="190"/>
+      <c r="H42" s="190"/>
+      <c r="I42" s="190"/>
     </row>
     <row r="43" spans="1:10" s="9" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="183" t="s">
+      <c r="A43" s="191" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="184"/>
-      <c r="C43" s="184"/>
-      <c r="D43" s="197" t="s">
+      <c r="B43" s="192"/>
+      <c r="C43" s="192"/>
+      <c r="D43" s="188" t="s">
         <v>53</v>
       </c>
-      <c r="E43" s="197"/>
-      <c r="F43" s="197"/>
-      <c r="G43" s="197"/>
-      <c r="H43" s="197"/>
-      <c r="I43" s="197"/>
+      <c r="E43" s="188"/>
+      <c r="F43" s="188"/>
+      <c r="G43" s="188"/>
+      <c r="H43" s="188"/>
+      <c r="I43" s="188"/>
     </row>
     <row r="44" spans="1:10" s="9" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="196" t="s">
+      <c r="A44" s="187" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="196"/>
-      <c r="C44" s="196"/>
-      <c r="D44" s="194" t="str">
+      <c r="B44" s="187"/>
+      <c r="C44" s="187"/>
+      <c r="D44" s="185" t="str">
         <f>'PC 1'!B68</f>
         <v>Alawiye, K.T (Ms)</v>
       </c>
-      <c r="E44" s="194"/>
-      <c r="F44" s="194"/>
-      <c r="G44" s="194"/>
-      <c r="H44" s="194"/>
-      <c r="I44" s="194"/>
+      <c r="E44" s="185"/>
+      <c r="F44" s="185"/>
+      <c r="G44" s="185"/>
+      <c r="H44" s="185"/>
+      <c r="I44" s="185"/>
     </row>
     <row r="45" spans="1:10" s="9" customFormat="1" ht="22.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="196" t="s">
+      <c r="A45" s="187" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="196"/>
-      <c r="C45" s="196"/>
-      <c r="D45" s="194" t="str">
+      <c r="B45" s="187"/>
+      <c r="C45" s="187"/>
+      <c r="D45" s="185" t="str">
         <f>'PC 1'!B69</f>
         <v>PPO (MED)</v>
       </c>
-      <c r="E45" s="194"/>
-      <c r="F45" s="194"/>
-      <c r="G45" s="194"/>
-      <c r="H45" s="194"/>
-      <c r="I45" s="194"/>
+      <c r="E45" s="185"/>
+      <c r="F45" s="185"/>
+      <c r="G45" s="185"/>
+      <c r="H45" s="185"/>
+      <c r="I45" s="185"/>
     </row>
     <row r="46" spans="1:10" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="181"/>
-      <c r="B46" s="181"/>
-      <c r="C46" s="181"/>
-      <c r="D46" s="186">
+      <c r="A46" s="196"/>
+      <c r="B46" s="196"/>
+      <c r="C46" s="196"/>
+      <c r="D46" s="199">
         <f>'PC 1'!B36</f>
         <v>0</v>
       </c>
-      <c r="E46" s="186"/>
-      <c r="F46" s="186"/>
-      <c r="G46" s="186"/>
-      <c r="H46" s="186"/>
-      <c r="I46" s="186"/>
+      <c r="E46" s="199"/>
+      <c r="F46" s="199"/>
+      <c r="G46" s="199"/>
+      <c r="H46" s="199"/>
+      <c r="I46" s="199"/>
       <c r="J46" s="12"/>
     </row>
     <row r="47" spans="1:10" s="9" customFormat="1" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="182"/>
-      <c r="B47" s="182"/>
-      <c r="C47" s="182"/>
-      <c r="D47" s="182"/>
-      <c r="E47" s="182"/>
-      <c r="F47" s="182"/>
-      <c r="G47" s="182"/>
-      <c r="H47" s="182"/>
+      <c r="A47" s="197"/>
+      <c r="B47" s="197"/>
+      <c r="C47" s="197"/>
+      <c r="D47" s="197"/>
+      <c r="E47" s="197"/>
+      <c r="F47" s="197"/>
+      <c r="G47" s="197"/>
+      <c r="H47" s="197"/>
     </row>
     <row r="48" spans="1:10" s="9" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="182"/>
-      <c r="B48" s="182"/>
-      <c r="C48" s="182"/>
-      <c r="D48" s="182"/>
-      <c r="E48" s="182"/>
-      <c r="F48" s="182"/>
-      <c r="G48" s="182"/>
-      <c r="H48" s="182"/>
+      <c r="A48" s="197"/>
+      <c r="B48" s="197"/>
+      <c r="C48" s="197"/>
+      <c r="D48" s="197"/>
+      <c r="E48" s="197"/>
+      <c r="F48" s="197"/>
+      <c r="G48" s="197"/>
+      <c r="H48" s="197"/>
     </row>
     <row r="49" spans="1:9" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="183" t="s">
+      <c r="A49" s="191" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="184"/>
-      <c r="C49" s="185" t="s">
+      <c r="B49" s="192"/>
+      <c r="C49" s="198" t="s">
         <v>100</v>
       </c>
-      <c r="D49" s="182"/>
-      <c r="E49" s="187" t="s">
+      <c r="D49" s="197"/>
+      <c r="E49" s="200" t="s">
         <v>100</v>
       </c>
-      <c r="F49" s="187"/>
-      <c r="G49" s="187"/>
-      <c r="H49" s="187"/>
-      <c r="I49" s="187"/>
+      <c r="F49" s="200"/>
+      <c r="G49" s="200"/>
+      <c r="H49" s="200"/>
+      <c r="I49" s="200"/>
     </row>
     <row r="50" spans="1:9" s="10" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="179" t="s">
+      <c r="A50" s="194" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="179"/>
-      <c r="C50" s="180" t="s">
+      <c r="B50" s="194"/>
+      <c r="C50" s="195" t="s">
         <v>96</v>
       </c>
-      <c r="D50" s="180"/>
-      <c r="E50" s="188" t="s">
+      <c r="D50" s="195"/>
+      <c r="E50" s="180" t="s">
         <v>97</v>
       </c>
-      <c r="F50" s="188"/>
-      <c r="G50" s="188"/>
-      <c r="H50" s="188"/>
-      <c r="I50" s="188"/>
+      <c r="F50" s="180"/>
+      <c r="G50" s="180"/>
+      <c r="H50" s="180"/>
+      <c r="I50" s="180"/>
     </row>
     <row r="51" spans="1:9" s="10" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="179" t="s">
+      <c r="A51" s="194" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="179"/>
-      <c r="C51" s="180" t="s">
+      <c r="B51" s="194"/>
+      <c r="C51" s="195" t="s">
         <v>99</v>
       </c>
-      <c r="D51" s="180"/>
-      <c r="E51" s="188" t="s">
+      <c r="D51" s="195"/>
+      <c r="E51" s="180" t="s">
         <v>101</v>
       </c>
-      <c r="F51" s="188"/>
-      <c r="G51" s="188"/>
-      <c r="H51" s="188"/>
-      <c r="I51" s="188"/>
+      <c r="F51" s="180"/>
+      <c r="G51" s="180"/>
+      <c r="H51" s="180"/>
+      <c r="I51" s="180"/>
     </row>
     <row r="52" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="53" spans="1:9" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="54" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wSi01L1jKFu+/KQxITGp8tiq0szckHTaxzJLu072ahrMN6+Ye2bpNLJt+by28nnvUGN3JJff6DAJRDUOkK4L2A==" saltValue="nV0vD9TDN1ZfxYMKAhZBXQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="v6m4mPDwyXr13VqojPTYvJAvuR8Sxunwk9MVy9weiXTdN/wNrDpr6NXTcB2z3V+cirn7DWrhm/ffLGYx4An/RA==" saltValue="RPUr62RzvjQ0Ucl318luZw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="56">
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="C17:I17"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="A38:I40"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:I51"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:I46"/>
+    <mergeCell ref="A47:H48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:I49"/>
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="C50:D50"/>
@@ -9222,46 +8752,6 @@
     <mergeCell ref="B35:I35"/>
     <mergeCell ref="B36:I36"/>
     <mergeCell ref="A37:I37"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E51:I51"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:I46"/>
-    <mergeCell ref="A47:H48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:I49"/>
-    <mergeCell ref="A38:I40"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="C19:I19"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C15:I15"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="C17:I17"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -9295,63 +8785,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="135" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="227" t="s">
+      <c r="A1" s="204" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="227"/>
-      <c r="C1" s="227"/>
-      <c r="D1" s="227"/>
-      <c r="E1" s="227"/>
-      <c r="F1" s="227"/>
-      <c r="G1" s="227"/>
-      <c r="H1" s="227"/>
+      <c r="B1" s="204"/>
+      <c r="C1" s="204"/>
+      <c r="D1" s="204"/>
+      <c r="E1" s="204"/>
+      <c r="F1" s="204"/>
+      <c r="G1" s="204"/>
+      <c r="H1" s="204"/>
     </row>
     <row r="2" spans="1:8" s="135" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="227" t="s">
+      <c r="A2" s="204" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="227"/>
-      <c r="C2" s="227"/>
-      <c r="D2" s="227"/>
-      <c r="E2" s="227"/>
-      <c r="F2" s="227"/>
-      <c r="G2" s="227"/>
-      <c r="H2" s="227"/>
+      <c r="B2" s="204"/>
+      <c r="C2" s="204"/>
+      <c r="D2" s="204"/>
+      <c r="E2" s="204"/>
+      <c r="F2" s="204"/>
+      <c r="G2" s="204"/>
+      <c r="H2" s="204"/>
     </row>
     <row r="3" spans="1:8" s="135" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A3" s="227" t="s">
+      <c r="A3" s="204" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="227"/>
-      <c r="C3" s="227"/>
-      <c r="D3" s="227"/>
-      <c r="E3" s="227"/>
-      <c r="F3" s="227"/>
-      <c r="G3" s="227"/>
-      <c r="H3" s="227"/>
+      <c r="B3" s="204"/>
+      <c r="C3" s="204"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="204"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
     </row>
     <row r="4" spans="1:8" s="135" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="228"/>
-      <c r="B4" s="228"/>
-      <c r="C4" s="228"/>
-      <c r="D4" s="228"/>
-      <c r="E4" s="228"/>
-      <c r="F4" s="228"/>
-      <c r="G4" s="228"/>
-      <c r="H4" s="228"/>
+      <c r="A4" s="214"/>
+      <c r="B4" s="214"/>
+      <c r="C4" s="214"/>
+      <c r="D4" s="214"/>
+      <c r="E4" s="214"/>
+      <c r="F4" s="214"/>
+      <c r="G4" s="214"/>
+      <c r="H4" s="214"/>
     </row>
     <row r="5" spans="1:8" s="136" customFormat="1" ht="99.6" customHeight="1" x14ac:dyDescent="0.85">
       <c r="A5" s="137" t="s">
         <v>173</v>
       </c>
-      <c r="B5" s="229">
+      <c r="B5" s="215">
         <f>'PC 1'!B23</f>
         <v>0</v>
       </c>
-      <c r="C5" s="229"/>
-      <c r="D5" s="229"/>
-      <c r="E5" s="229"/>
-      <c r="F5" s="229"/>
+      <c r="C5" s="215"/>
+      <c r="D5" s="215"/>
+      <c r="E5" s="215"/>
+      <c r="F5" s="215"/>
       <c r="G5" s="137" t="s">
         <v>118</v>
       </c>
@@ -9364,14 +8854,14 @@
       <c r="A6" s="137" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="229">
+      <c r="B6" s="215">
         <f>'PC 2'!B23</f>
         <v>0</v>
       </c>
-      <c r="C6" s="229"/>
-      <c r="D6" s="229"/>
-      <c r="E6" s="229"/>
-      <c r="F6" s="229"/>
+      <c r="C6" s="215"/>
+      <c r="D6" s="215"/>
+      <c r="E6" s="215"/>
+      <c r="F6" s="215"/>
       <c r="G6" s="137"/>
       <c r="H6" s="167"/>
     </row>
@@ -9379,14 +8869,14 @@
       <c r="A7" s="137" t="s">
         <v>174</v>
       </c>
-      <c r="B7" s="229">
+      <c r="B7" s="215">
         <f>'PC 1'!B20</f>
         <v>0</v>
       </c>
-      <c r="C7" s="229"/>
-      <c r="D7" s="229"/>
-      <c r="E7" s="229"/>
-      <c r="F7" s="229"/>
+      <c r="C7" s="215"/>
+      <c r="D7" s="215"/>
+      <c r="E7" s="215"/>
+      <c r="F7" s="215"/>
       <c r="G7" s="138" t="s">
         <v>176</v>
       </c>
@@ -9399,14 +8889,14 @@
       <c r="A8" s="137" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="230" t="str">
+      <c r="B8" s="205" t="str">
         <f>'PC 1'!B28&amp;" "&amp;"/"&amp;'PC 2'!B28</f>
         <v>0 /0</v>
       </c>
-      <c r="C8" s="230"/>
-      <c r="D8" s="230"/>
-      <c r="E8" s="230"/>
-      <c r="F8" s="230"/>
+      <c r="C8" s="205"/>
+      <c r="D8" s="205"/>
+      <c r="E8" s="205"/>
+      <c r="F8" s="205"/>
       <c r="G8" s="138" t="s">
         <v>218</v>
       </c>
@@ -9419,14 +8909,14 @@
       <c r="A9" s="137" t="s">
         <v>221</v>
       </c>
-      <c r="B9" s="231" t="str">
+      <c r="B9" s="206" t="str">
         <f>'PC 1'!B22 &amp; "/" &amp; 'PC 2'!B22</f>
         <v>0/0</v>
       </c>
-      <c r="C9" s="231"/>
-      <c r="D9" s="231"/>
-      <c r="E9" s="231"/>
-      <c r="F9" s="231"/>
+      <c r="C9" s="206"/>
+      <c r="D9" s="206"/>
+      <c r="E9" s="206"/>
+      <c r="F9" s="206"/>
       <c r="G9" s="138" t="s">
         <v>113</v>
       </c>
@@ -9438,14 +8928,14 @@
       <c r="A10" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="230">
+      <c r="B10" s="205">
         <f>'PC 1'!B21</f>
         <v>0</v>
       </c>
-      <c r="C10" s="230"/>
-      <c r="D10" s="230"/>
-      <c r="E10" s="230"/>
-      <c r="F10" s="230"/>
+      <c r="C10" s="205"/>
+      <c r="D10" s="205"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="205"/>
       <c r="G10" s="138" t="s">
         <v>177</v>
       </c>
@@ -9458,51 +8948,51 @@
       <c r="A11" s="137" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="230" t="s">
+      <c r="B11" s="205" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="230"/>
-      <c r="D11" s="230"/>
-      <c r="E11" s="230"/>
-      <c r="F11" s="230"/>
+      <c r="C11" s="205"/>
+      <c r="D11" s="205"/>
+      <c r="E11" s="205"/>
+      <c r="F11" s="205"/>
       <c r="G11" s="169"/>
       <c r="H11" s="169"/>
     </row>
     <row r="12" spans="1:8" s="136" customFormat="1" ht="49.2" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A12" s="227"/>
-      <c r="B12" s="227"/>
-      <c r="C12" s="227"/>
-      <c r="D12" s="227"/>
-      <c r="E12" s="227"/>
-      <c r="F12" s="227"/>
-      <c r="G12" s="227"/>
-      <c r="H12" s="227"/>
+      <c r="A12" s="204"/>
+      <c r="B12" s="204"/>
+      <c r="C12" s="204"/>
+      <c r="D12" s="204"/>
+      <c r="E12" s="204"/>
+      <c r="F12" s="204"/>
+      <c r="G12" s="204"/>
+      <c r="H12" s="204"/>
     </row>
     <row r="13" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A13" s="232" t="s">
+      <c r="A13" s="207" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="205"/>
-      <c r="C13" s="205"/>
-      <c r="D13" s="233"/>
+      <c r="B13" s="208"/>
+      <c r="C13" s="208"/>
+      <c r="D13" s="209"/>
       <c r="E13" s="134" t="s">
         <v>59</v>
       </c>
       <c r="F13" s="134" t="s">
         <v>151</v>
       </c>
-      <c r="G13" s="201" t="s">
+      <c r="G13" s="210" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="202"/>
+      <c r="H13" s="211"/>
     </row>
     <row r="14" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A14" s="218" t="s">
+      <c r="A14" s="201" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="219"/>
-      <c r="C14" s="219"/>
-      <c r="D14" s="220"/>
+      <c r="B14" s="202"/>
+      <c r="C14" s="202"/>
+      <c r="D14" s="203"/>
       <c r="E14" s="140" t="s">
         <v>122</v>
       </c>
@@ -9514,12 +9004,12 @@
       <c r="H14" s="213"/>
     </row>
     <row r="15" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A15" s="218" t="s">
+      <c r="A15" s="201" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="219"/>
-      <c r="C15" s="219"/>
-      <c r="D15" s="220"/>
+      <c r="B15" s="202"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="203"/>
       <c r="E15" s="140" t="s">
         <v>122</v>
       </c>
@@ -9531,12 +9021,12 @@
       <c r="H15" s="213"/>
     </row>
     <row r="16" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A16" s="218" t="s">
+      <c r="A16" s="201" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="219"/>
-      <c r="C16" s="219"/>
-      <c r="D16" s="220"/>
+      <c r="B16" s="202"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="203"/>
       <c r="E16" s="140" t="s">
         <v>122</v>
       </c>
@@ -9548,12 +9038,12 @@
       <c r="H16" s="213"/>
     </row>
     <row r="17" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A17" s="218" t="s">
+      <c r="A17" s="201" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="219"/>
-      <c r="C17" s="219"/>
-      <c r="D17" s="220"/>
+      <c r="B17" s="202"/>
+      <c r="C17" s="202"/>
+      <c r="D17" s="203"/>
       <c r="E17" s="140" t="s">
         <v>122</v>
       </c>
@@ -9565,13 +9055,13 @@
       <c r="H17" s="213"/>
     </row>
     <row r="18" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A18" s="218">
+      <c r="A18" s="201">
         <f>'PC 1'!B37</f>
         <v>0</v>
       </c>
-      <c r="B18" s="219"/>
-      <c r="C18" s="219"/>
-      <c r="D18" s="220"/>
+      <c r="B18" s="202"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="203"/>
       <c r="E18" s="140" t="s">
         <v>122</v>
       </c>
@@ -9583,12 +9073,12 @@
       <c r="H18" s="213"/>
     </row>
     <row r="19" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A19" s="218" t="s">
+      <c r="A19" s="201" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="219"/>
-      <c r="C19" s="219"/>
-      <c r="D19" s="220"/>
+      <c r="B19" s="202"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="203"/>
       <c r="E19" s="140"/>
       <c r="F19" s="140" t="s">
         <v>122</v>
@@ -9600,12 +9090,12 @@
       <c r="H19" s="213"/>
     </row>
     <row r="20" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A20" s="218" t="s">
+      <c r="A20" s="201" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="219"/>
-      <c r="C20" s="219"/>
-      <c r="D20" s="220"/>
+      <c r="B20" s="202"/>
+      <c r="C20" s="202"/>
+      <c r="D20" s="203"/>
       <c r="E20" s="140"/>
       <c r="F20" s="140" t="s">
         <v>122</v>
@@ -9617,12 +9107,12 @@
       <c r="H20" s="213"/>
     </row>
     <row r="21" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A21" s="218" t="s">
+      <c r="A21" s="201" t="s">
         <v>181</v>
       </c>
-      <c r="B21" s="219"/>
-      <c r="C21" s="219"/>
-      <c r="D21" s="220"/>
+      <c r="B21" s="202"/>
+      <c r="C21" s="202"/>
+      <c r="D21" s="203"/>
       <c r="E21" s="140"/>
       <c r="F21" s="140"/>
       <c r="G21" s="212" t="str">
@@ -9632,12 +9122,12 @@
       <c r="H21" s="213"/>
     </row>
     <row r="22" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A22" s="218" t="s">
+      <c r="A22" s="201" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="219"/>
-      <c r="C22" s="219"/>
-      <c r="D22" s="220"/>
+      <c r="B22" s="202"/>
+      <c r="C22" s="202"/>
+      <c r="D22" s="203"/>
       <c r="E22" s="141"/>
       <c r="F22" s="140" t="s">
         <v>122</v>
@@ -9649,12 +9139,12 @@
       <c r="H22" s="213"/>
     </row>
     <row r="23" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A23" s="218" t="s">
+      <c r="A23" s="201" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="226"/>
-      <c r="C23" s="219"/>
-      <c r="D23" s="220"/>
+      <c r="B23" s="222"/>
+      <c r="C23" s="202"/>
+      <c r="D23" s="203"/>
       <c r="E23" s="143"/>
       <c r="F23" s="143"/>
       <c r="G23" s="212" t="str">
@@ -9667,35 +9157,35 @@
       <c r="A24" s="142" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="221" t="str">
+      <c r="B24" s="217" t="str">
         <f>'PC 1'!B25 &amp; "/" &amp; 'PC 2'!B25</f>
         <v>0/0</v>
       </c>
-      <c r="C24" s="221"/>
-      <c r="D24" s="221"/>
-      <c r="E24" s="221"/>
-      <c r="F24" s="221"/>
-      <c r="G24" s="221"/>
-      <c r="H24" s="222"/>
+      <c r="C24" s="217"/>
+      <c r="D24" s="217"/>
+      <c r="E24" s="217"/>
+      <c r="F24" s="217"/>
+      <c r="G24" s="217"/>
+      <c r="H24" s="218"/>
     </row>
     <row r="25" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A25" s="201" t="s">
+      <c r="A25" s="210" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="223"/>
-      <c r="C25" s="223"/>
-      <c r="D25" s="223"/>
+      <c r="B25" s="219"/>
+      <c r="C25" s="219"/>
+      <c r="D25" s="219"/>
       <c r="E25" s="146"/>
       <c r="F25" s="146"/>
-      <c r="G25" s="224"/>
-      <c r="H25" s="225"/>
+      <c r="G25" s="220"/>
+      <c r="H25" s="221"/>
     </row>
     <row r="26" spans="1:8" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A26" s="212" t="s">
         <v>124</v>
       </c>
-      <c r="B26" s="214"/>
-      <c r="C26" s="214"/>
+      <c r="B26" s="216"/>
+      <c r="C26" s="216"/>
       <c r="D26" s="213"/>
       <c r="E26" s="144"/>
       <c r="F26" s="144"/>
@@ -9708,8 +9198,8 @@
       <c r="A27" s="212" t="s">
         <v>123</v>
       </c>
-      <c r="B27" s="214"/>
-      <c r="C27" s="214"/>
+      <c r="B27" s="216"/>
+      <c r="C27" s="216"/>
       <c r="D27" s="213"/>
       <c r="E27" s="144"/>
       <c r="F27" s="144"/>
@@ -9722,8 +9212,8 @@
       <c r="A28" s="212" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="214"/>
-      <c r="C28" s="214"/>
+      <c r="B28" s="216"/>
+      <c r="C28" s="216"/>
       <c r="D28" s="213"/>
       <c r="E28" s="144"/>
       <c r="F28" s="144"/>
@@ -9736,8 +9226,8 @@
       <c r="A29" s="212" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="214"/>
-      <c r="C29" s="214"/>
+      <c r="B29" s="216"/>
+      <c r="C29" s="216"/>
       <c r="D29" s="213"/>
       <c r="E29" s="144"/>
       <c r="F29" s="144"/>
@@ -9750,8 +9240,8 @@
       <c r="A30" s="212" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="214"/>
-      <c r="C30" s="214"/>
+      <c r="B30" s="216"/>
+      <c r="C30" s="216"/>
       <c r="D30" s="213"/>
       <c r="E30" s="144"/>
       <c r="F30" s="144"/>
@@ -9762,8 +9252,8 @@
       <c r="A31" s="212" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="214"/>
-      <c r="C31" s="214"/>
+      <c r="B31" s="216"/>
+      <c r="C31" s="216"/>
       <c r="D31" s="213"/>
       <c r="E31" s="144"/>
       <c r="F31" s="144"/>
@@ -9777,8 +9267,8 @@
       <c r="A32" s="212" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="214"/>
-      <c r="C32" s="214"/>
+      <c r="B32" s="216"/>
+      <c r="C32" s="216"/>
       <c r="D32" s="213"/>
       <c r="E32" s="144"/>
       <c r="F32" s="144"/>
@@ -9789,24 +9279,24 @@
       <c r="H32" s="213"/>
     </row>
     <row r="33" spans="1:10" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A33" s="215" t="s">
+      <c r="A33" s="223" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="216"/>
-      <c r="C33" s="216"/>
-      <c r="D33" s="217"/>
+      <c r="B33" s="224"/>
+      <c r="C33" s="224"/>
+      <c r="D33" s="225"/>
       <c r="E33" s="144"/>
       <c r="F33" s="144"/>
       <c r="G33" s="212"/>
       <c r="H33" s="213"/>
     </row>
     <row r="34" spans="1:10" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A34" s="210" t="s">
+      <c r="A34" s="226" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="210"/>
-      <c r="C34" s="210"/>
-      <c r="D34" s="210"/>
+      <c r="B34" s="226"/>
+      <c r="C34" s="226"/>
+      <c r="D34" s="226"/>
       <c r="E34" s="145" t="s">
         <v>122</v>
       </c>
@@ -9815,50 +9305,50 @@
       <c r="H34" s="213"/>
     </row>
     <row r="35" spans="1:10" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A35" s="210" t="s">
+      <c r="A35" s="226" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="210"/>
-      <c r="C35" s="210"/>
-      <c r="D35" s="210"/>
+      <c r="B35" s="226"/>
+      <c r="C35" s="226"/>
+      <c r="D35" s="226"/>
       <c r="E35" s="145"/>
       <c r="F35" s="144"/>
       <c r="G35" s="212"/>
       <c r="H35" s="213"/>
     </row>
     <row r="36" spans="1:10" s="136" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A36" s="209" t="s">
+      <c r="A36" s="227" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="209"/>
-      <c r="C36" s="209"/>
-      <c r="D36" s="209"/>
+      <c r="B36" s="227"/>
+      <c r="C36" s="227"/>
+      <c r="D36" s="227"/>
       <c r="E36" s="145"/>
       <c r="F36" s="144"/>
       <c r="G36" s="212"/>
       <c r="H36" s="213"/>
     </row>
     <row r="37" spans="1:10" s="136" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A37" s="210" t="s">
+      <c r="A37" s="226" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="210"/>
-      <c r="C37" s="210"/>
-      <c r="D37" s="210"/>
+      <c r="B37" s="226"/>
+      <c r="C37" s="226"/>
+      <c r="D37" s="226"/>
       <c r="E37" s="145" t="s">
         <v>122</v>
       </c>
       <c r="F37" s="146"/>
-      <c r="G37" s="201"/>
-      <c r="H37" s="202"/>
+      <c r="G37" s="210"/>
+      <c r="H37" s="211"/>
     </row>
     <row r="38" spans="1:10" s="136" customFormat="1" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A38" s="211" t="s">
+      <c r="A38" s="228" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="210"/>
-      <c r="C38" s="210"/>
-      <c r="D38" s="210"/>
+      <c r="B38" s="226"/>
+      <c r="C38" s="226"/>
+      <c r="D38" s="226"/>
       <c r="E38" s="145" t="s">
         <v>122</v>
       </c>
@@ -9867,48 +9357,48 @@
       <c r="H38" s="213"/>
     </row>
     <row r="39" spans="1:10" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A39" s="208" t="s">
+      <c r="A39" s="233" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="208"/>
-      <c r="C39" s="208"/>
-      <c r="D39" s="206" t="str">
+      <c r="B39" s="233"/>
+      <c r="C39" s="233"/>
+      <c r="D39" s="231" t="str">
         <f>"Project 1: " &amp;'PC 1'!B33  &amp; " / " &amp;"Project 2: " &amp; 'PC 2'!B33</f>
         <v>Project 1: 0 / Project 2: 0</v>
       </c>
-      <c r="E39" s="206"/>
-      <c r="F39" s="206"/>
-      <c r="G39" s="206"/>
-      <c r="H39" s="207"/>
+      <c r="E39" s="231"/>
+      <c r="F39" s="231"/>
+      <c r="G39" s="231"/>
+      <c r="H39" s="232"/>
     </row>
     <row r="40" spans="1:10" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A40" s="205" t="s">
+      <c r="A40" s="208" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="205"/>
-      <c r="C40" s="205"/>
-      <c r="D40" s="206" t="str">
+      <c r="B40" s="208"/>
+      <c r="C40" s="208"/>
+      <c r="D40" s="231" t="str">
         <f>"Project 1: " &amp;'PC 1'!B34 &amp; " (satisfactory)" &amp; " / " &amp;"Project 2: " &amp; 'PC 2'!B34 &amp; " (satisfactory)"</f>
         <v>Project 1: 0 (satisfactory) / Project 2: 0 (satisfactory)</v>
       </c>
-      <c r="E40" s="206"/>
-      <c r="F40" s="206"/>
-      <c r="G40" s="206"/>
-      <c r="H40" s="207"/>
+      <c r="E40" s="231"/>
+      <c r="F40" s="231"/>
+      <c r="G40" s="231"/>
+      <c r="H40" s="232"/>
     </row>
     <row r="41" spans="1:10" s="136" customFormat="1" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A41" s="203" t="s">
+      <c r="A41" s="229" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="203"/>
-      <c r="C41" s="203"/>
-      <c r="D41" s="204"/>
+      <c r="B41" s="229"/>
+      <c r="C41" s="229"/>
+      <c r="D41" s="230"/>
       <c r="E41" s="140" t="s">
         <v>122</v>
       </c>
       <c r="F41" s="141"/>
-      <c r="G41" s="201"/>
-      <c r="H41" s="202"/>
+      <c r="G41" s="210"/>
+      <c r="H41" s="211"/>
       <c r="J41" s="147"/>
     </row>
     <row r="42" spans="1:10" s="136" customFormat="1" ht="2.4" customHeight="1" x14ac:dyDescent="0.85">
@@ -9956,53 +9446,12 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:H39"/>
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:D38"/>
@@ -10019,12 +9468,53 @@
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="D40:H40"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D39:H39"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="24" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>